<commit_message>
updating Weds/Thus schedule (affects ONLY MS)
</commit_message>
<xml_diff>
--- a/Detailed Company interview schedule.xlsx
+++ b/Detailed Company interview schedule.xlsx
@@ -683,8 +683,8 @@
   </sheetPr>
   <dimension ref="A1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H57" sqref="H57:H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,8 +692,8 @@
     <col min="1" max="1" width="8.5" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.5" style="1" customWidth="1"/>
     <col min="3" max="7" width="24" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.1640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="2.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="35.1640625" style="1" customWidth="1"/>
     <col min="10" max="13" width="10.83203125" style="2"/>
     <col min="14" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -1400,18 +1400,15 @@
         <v>55</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="E38" s="2" t="s">
+        <v>52</v>
+      </c>
       <c r="F38" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="G38" s="2" t="s">
         <v>48</v>
       </c>
       <c r="H38" s="1"/>
@@ -1425,18 +1422,15 @@
         <v>38</v>
       </c>
       <c r="C39" s="14" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D39" s="14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G39" s="14" t="s">
         <v>6</v>
       </c>
       <c r="H39" s="1"/>
@@ -1461,9 +1455,6 @@
       <c r="F40" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G40" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="21"/>
@@ -1475,18 +1466,15 @@
         <v>35</v>
       </c>
       <c r="C41" s="13" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G41" s="13" t="s">
         <v>34</v>
       </c>
       <c r="H41" s="1"/>
@@ -1511,9 +1499,6 @@
       <c r="F42" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G42" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="21"/>
@@ -1525,18 +1510,15 @@
         <v>30</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E43" s="16" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G43" s="16" t="s">
         <v>28</v>
       </c>
       <c r="H43" s="1"/>
@@ -1561,9 +1543,6 @@
       <c r="F44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G44" s="7" t="s">
-        <v>4</v>
-      </c>
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="21"/>
@@ -1575,18 +1554,15 @@
         <v>26</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D45" s="14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F45" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="G45" s="9" t="s">
+      <c r="F45" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H45" s="1"/>
@@ -1611,9 +1587,6 @@
       <c r="F46" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G46" s="7" t="s">
-        <v>10</v>
-      </c>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="21"/>
@@ -1625,18 +1598,15 @@
         <v>21</v>
       </c>
       <c r="C47" s="13" t="s">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="G47" s="5" t="s">
+      <c r="F47" s="5" t="s">
         <v>20</v>
       </c>
       <c r="H47" s="1"/>
@@ -1649,7 +1619,9 @@
       <c r="B48" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="D48" s="7" t="s">
         <v>4</v>
       </c>
@@ -1657,9 +1629,6 @@
         <v>4</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H48" s="1"/>
@@ -1672,17 +1641,16 @@
       <c r="B49" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11" t="s">
+      <c r="C49" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E49" s="16" t="s">
+      <c r="D49" s="16" t="s">
         <v>29</v>
       </c>
+      <c r="E49" s="11" t="s">
+        <v>34</v>
+      </c>
       <c r="F49" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G49" s="11" t="s">
         <v>13</v>
       </c>
       <c r="H49" s="1"/>
@@ -1695,7 +1663,9 @@
       <c r="B50" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="D50" s="7" t="s">
         <v>10</v>
       </c>
@@ -1703,9 +1673,6 @@
         <v>10</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="G50" s="7" t="s">
         <v>10</v>
       </c>
       <c r="H50" s="1"/>
@@ -1717,17 +1684,16 @@
       <c r="B51" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9" t="s">
+      <c r="C51" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E51" s="14" t="s">
+      <c r="D51" s="14" t="s">
         <v>28</v>
       </c>
+      <c r="E51" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="F51" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G51" s="9" t="s">
         <v>19</v>
       </c>
       <c r="H51" s="1"/>
@@ -1739,7 +1705,9 @@
       <c r="B52" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="7"/>
+      <c r="C52" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="D52" s="7" t="s">
         <v>4</v>
       </c>
@@ -1747,9 +1715,6 @@
         <v>4</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="G52" s="7" t="s">
         <v>4</v>
       </c>
       <c r="H52" s="1"/>
@@ -1761,17 +1726,16 @@
       <c r="B53" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5" t="s">
+      <c r="C53" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="D53" s="13" t="s">
         <v>37</v>
       </c>
+      <c r="E53" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="F53" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G53" s="5" t="s">
         <v>51</v>
       </c>
       <c r="H53" s="1"/>
@@ -1810,7 +1774,9 @@
       <c r="G56" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H56" s="1"/>
+      <c r="H56" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="I56" s="1"/>
       <c r="K56" s="4"/>
     </row>
@@ -1834,7 +1800,9 @@
       <c r="G57" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="H57" s="1"/>
+      <c r="H57" s="14" t="s">
+        <v>18</v>
+      </c>
       <c r="I57" s="1"/>
       <c r="J57" s="18"/>
       <c r="K57" s="4"/>
@@ -1859,7 +1827,9 @@
       <c r="G58" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H58" s="1"/>
+      <c r="H58" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="I58" s="1"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
@@ -1884,7 +1854,9 @@
       <c r="G59" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="H59" s="1"/>
+      <c r="H59" s="13" t="s">
+        <v>8</v>
+      </c>
       <c r="I59" s="1"/>
       <c r="J59" s="18"/>
       <c r="K59" s="4"/>
@@ -1909,7 +1881,9 @@
       <c r="G60" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H60" s="1"/>
+      <c r="H60" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="I60" s="1"/>
       <c r="J60" s="18"/>
       <c r="K60" s="4"/>
@@ -1934,7 +1908,9 @@
       <c r="G61" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="H61" s="1"/>
+      <c r="H61" s="16" t="s">
+        <v>29</v>
+      </c>
       <c r="I61" s="1"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
@@ -1959,7 +1935,9 @@
       <c r="G62" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H62" s="1"/>
+      <c r="H62" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="I62" s="1"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
@@ -1984,7 +1962,9 @@
       <c r="G63" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H63" s="1"/>
+      <c r="H63" s="14" t="s">
+        <v>28</v>
+      </c>
       <c r="I63" s="1"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
@@ -2009,7 +1989,9 @@
       <c r="G64" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H64" s="1"/>
+      <c r="H64" s="7" t="s">
+        <v>10</v>
+      </c>
       <c r="I64" s="1"/>
       <c r="J64" s="18"/>
     </row>
@@ -2033,7 +2015,9 @@
       <c r="G65" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H65" s="1"/>
+      <c r="H65" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2056,7 +2040,7 @@
       <c r="G66" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H66" s="1"/>
+      <c r="H66" s="7"/>
       <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2079,7 +2063,7 @@
       <c r="G67" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="H67" s="1"/>
+      <c r="H67" s="11"/>
       <c r="I67" s="1"/>
     </row>
     <row r="68" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2102,7 +2086,7 @@
       <c r="G68" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H68" s="1"/>
+      <c r="H68" s="7"/>
       <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2123,7 +2107,7 @@
         <v>6</v>
       </c>
       <c r="G69" s="9"/>
-      <c r="H69" s="1"/>
+      <c r="H69" s="9"/>
       <c r="I69" s="1"/>
     </row>
     <row r="70" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2146,7 +2130,7 @@
       <c r="G70" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="H70" s="1"/>
+      <c r="H70" s="7"/>
       <c r="I70" s="1"/>
     </row>
     <row r="71" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -2167,7 +2151,7 @@
         <v>34</v>
       </c>
       <c r="G71" s="5"/>
-      <c r="H71" s="1"/>
+      <c r="H71" s="5"/>
       <c r="I71" s="1"/>
     </row>
     <row r="74" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>